<commit_message>
Use case diagram/template en notulen
</commit_message>
<xml_diff>
--- a/Barroc IT - Documentatie/Steven/Group 1 - Notulen - 05-10-2015/Notulen 05-10-2015 (v2).xlsx
+++ b/Barroc IT - Documentatie/Steven/Group 1 - Notulen - 05-10-2015/Notulen 05-10-2015 (v2).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Afwezig:</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>Tom</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>12.2</t>
+  </si>
+  <si>
+    <t>12.3</t>
+  </si>
+  <si>
+    <t>Groep 1</t>
   </si>
 </sst>
 </file>
@@ -342,7 +354,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>594361</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -668,7 +680,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,11 +692,13 @@
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -1005,8 +1019,8 @@
       <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="26">
-        <v>13</v>
+      <c r="A19" s="26" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>25</v>
@@ -1016,8 +1030,8 @@
       <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="26">
-        <v>14</v>
+      <c r="A20" s="26" t="s">
+        <v>37</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>26</v>
@@ -1027,8 +1041,8 @@
       <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="26">
-        <v>15</v>
+      <c r="A21" s="26" t="s">
+        <v>38</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>27</v>
@@ -1038,9 +1052,7 @@
       <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="26">
-        <v>16</v>
-      </c>
+      <c r="A22" s="26"/>
       <c r="B22" s="19"/>
       <c r="C22" s="14"/>
       <c r="D22" s="15"/>
@@ -1123,6 +1135,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8428B090D81B34DA19517DD6F855647" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="461551752daf7baccd316804784cc5e1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b118b0825d757084c8d1e1ffd33f200c">
     <xsd:element name="properties">
@@ -1171,12 +1189,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1187,6 +1199,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F91946DA-1D0C-4852-AC5F-029A4620CB68}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{579EC409-788A-470F-B358-7D465288959E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1201,20 +1227,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F91946DA-1D0C-4852-AC5F-029A4620CB68}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79336D9A-F347-4BF9-A03C-2F519BF74106}">
   <ds:schemaRefs>

</xml_diff>